<commit_message>
r add pll and rti
</commit_message>
<xml_diff>
--- a/docs/semiconductors/section2/topic1/assets/a-BJT.xlsx
+++ b/docs/semiconductors/section2/topic1/assets/a-BJT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\a-Computer-Engineering\Semiconductors-Private\j-Transistor-Applications\a-BJTs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbinl\Documents\GitHub\CMPE1400\j-Transistor-Applications\a-BJTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6218A6EA-42BD-40F0-9BC1-AA0872E89B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1463C8-9E02-4E20-B9C5-E7D3DC0A4AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="877" xr2:uid="{E80DF3CB-22C8-48CC-A275-866A023A71E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="877" xr2:uid="{E80DF3CB-22C8-48CC-A275-866A023A71E1}"/>
   </bookViews>
   <sheets>
     <sheet name="L-Models-NPN-Active" sheetId="25" r:id="rId1"/>
@@ -2468,7 +2468,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>3625857</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>195693</xdr:rowOff>
+      <xdr:rowOff>186168</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3169,23 +3169,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277585F0-62A0-47EC-B022-A79255249C20}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.3984375" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3392,83 +3392,83 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="6"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" s="7"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="7"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="7"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="7"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="7"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E37" s="4"/>
     </row>
   </sheetData>
@@ -3481,23 +3481,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDE9E55-60C4-4CC7-B7F9-F6F05C50A3F8}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.3984375" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -3559,33 +3559,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="str">
-        <f>TEXT(20,"0.00")</f>
-        <v>20.00</v>
+        <f>TEXT(15,"0.00")</f>
+        <v>15.00</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="str">
-        <f>TEXT(10,"0.00")</f>
-        <v>10.00</v>
+        <f>TEXT(5,"0.00")</f>
+        <v>5.00</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="D7" s="8" t="str">
         <f>TEXT(680,"##0E+0")</f>
@@ -3595,7 +3595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3607,27 +3607,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1" t="str">
         <f>_xlfn.CONCAT("(",A5,"-",A3,")/",A7)</f>
-        <v>(VCC-VECsat)/Re_given</v>
+        <v>(VCC-VECsat)/Rc_given</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>_xlfn.CONCAT("(",D5,"-",D3,")/",D7)</f>
-        <v>(20.00-0.30)/680E+0</v>
+        <v>(15.00-0.30)/680E+0</v>
       </c>
       <c r="D10" s="8" t="str">
         <f>TEXT((D5-D3)/(D7),"##0.0E+0")</f>
-        <v>29.0E-3</v>
+        <v>21.6E-3</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3636,12 +3636,12 @@
         <v>(VCC-VEB_on-VBB)/Rb_given</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f>_xlfn.CONCAT("(",D6,"-",D4,")/",D8)</f>
-        <v>(10.00-0.70)/100E+3</v>
+        <f>_xlfn.CONCAT("(",D5,"-",D4,"-",D6,")/",D8)</f>
+        <v>(15.00-0.70-5.00)/100E+3</v>
       </c>
       <c r="D11" s="26" t="str">
         <f>TEXT((D6-D4)/(D8),"##0.0E+0")</f>
-        <v>93.0E-6</v>
+        <v>43.0E-6</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
@@ -3650,7 +3650,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3660,17 +3660,17 @@
       </c>
       <c r="C12" s="1" t="str">
         <f>_xlfn.CONCAT(D11,"*",D2)</f>
-        <v>93.0E-6*130</v>
+        <v>43.0E-6*130</v>
       </c>
       <c r="D12" s="8" t="str">
         <f>TEXT(D11*D2,"##0.00E+0")</f>
-        <v>12.09E-3</v>
+        <v>5.59E-3</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -3679,7 +3679,7 @@
       </c>
       <c r="D13" s="26" t="str">
         <f>TEXT(IF(D12-D10&gt;0,D10,D12),"##0.00E+0")</f>
-        <v>12.09E-3</v>
+        <v>5.59E-3</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
@@ -3688,7 +3688,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3707,83 +3707,83 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="6"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" s="7"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="7"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="7"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="7"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="7"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E37" s="4"/>
     </row>
   </sheetData>
@@ -3796,23 +3796,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8688BD-BC2D-4011-B749-B74D690D114E}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.3984375" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4019,83 +4019,83 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="6"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" s="7"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="7"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="7"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="7"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="7"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E37" s="4"/>
     </row>
   </sheetData>
@@ -4112,19 +4112,19 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.44921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1484375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.44921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67.3984375" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>100.00</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4328,83 +4328,83 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="6"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" s="7"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D32" s="7"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="7"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="7"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="7"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E37" s="4"/>
     </row>
   </sheetData>
@@ -4421,19 +4421,19 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.84765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>100.00</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4537,10 +4537,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
@@ -4671,83 +4671,83 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D19" s="10"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D20" s="11"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D21" s="10"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D22" s="10"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D25" s="16"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D26" s="10"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D27" s="10"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D28" s="10"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D30" s="17"/>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D31" s="18"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.6">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D32" s="18"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="18"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="18"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="18"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="18"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="18"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E38" s="15"/>
     </row>
   </sheetData>
@@ -4765,19 +4765,19 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.34765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.84765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="106.046875" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="106" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>1.9609999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>1.0330000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -4884,7 +4884,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -4908,10 +4908,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -5187,77 +5187,77 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D30" s="11"/>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D31" s="10"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D32" s="10"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="10"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="17"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="18"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="18"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="18"/>
       <c r="E38" s="15"/>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" s="18"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D40" s="18"/>
       <c r="E40" s="15"/>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D41" s="18"/>
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D42" s="18"/>
       <c r="E42" s="15"/>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E43" s="15"/>
     </row>
   </sheetData>
@@ -5274,20 +5274,20 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.84765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="88.5" customWidth="1"/>
-    <col min="9" max="9" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -5338,7 +5338,7 @@
         <v>1.3610000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>7.0699999999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>6.8100000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -5448,10 +5448,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -5551,7 +5551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -5591,7 +5591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -5631,79 +5631,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D25" s="11"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D26" s="11"/>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D27" s="11"/>
       <c r="E27" s="15"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D28" s="11"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D29" s="10"/>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D30" s="10"/>
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D32" s="17"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" s="18"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" s="18"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" s="18"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" s="18"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="18"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="18"/>
       <c r="E38" s="15"/>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" s="18"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.6">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E40" s="15"/>
     </row>
   </sheetData>

</xml_diff>